<commit_message>
fix issue in word and inconsist version
</commit_message>
<xml_diff>
--- a/public/download/format-user-import.xlsx
+++ b/public/download/format-user-import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\firdaus\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7420C4D-D30A-434D-9C79-AF2971103699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8143DE7C-3D21-B546-B28F-01DD5CE3AA7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{5B61C8D2-81D4-40EA-81DF-8566B3E2BCD4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20740" windowHeight="11320" xr2:uid="{5B61C8D2-81D4-40EA-81DF-8566B3E2BCD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,8 +30,45 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{DA4E14AC-1822-E143-8BAB-7C13261BAD5F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Terdapat 3 role:
+admin
+operator
+guru</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">Nama </t>
   </si>
@@ -41,12 +78,15 @@
   <si>
     <t>Password</t>
   </si>
+  <si>
+    <t>Role</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +111,19 @@
       <family val="2"/>
       <charset val="1"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -418,21 +471,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B49708-2546-43AA-AE4D-C9D3B47182A5}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B49708-2546-43AA-AE4D-C9D3B47182A5}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -442,11 +495,15 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>